<commit_message>
added check in and out functionality
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1192,12 +1192,12 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 15</t>
+          <t xml:space="preserve"> Desk</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 15</t>
+          <t xml:space="preserve"> Main Desktop</t>
         </is>
       </c>
     </row>
@@ -1354,6 +1354,162 @@
       <c r="J18" t="inlineStr">
         <is>
           <t xml:space="preserve"> 21</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>119</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans1</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans1</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans1</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans1</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans1</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans1</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans1</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans2</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans2</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans3_1</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans3_1</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans3_1</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans3_1</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans3_1</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans3_1</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans3_1</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Storage_1</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N/A_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>121</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans3_1</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans3_1</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans3_1</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans3_1</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans3_1</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans3_1</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans3_1</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Storage</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N/A</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
begin conversion to multiple windows
redesigning user interface to have separate windows for each function

tkinter-window.py is the targeted window framework
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -413,14 +413,1159 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>101</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>102</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 3</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 3</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 3</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 3</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 3</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 3</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 3</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 3</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>103</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 4</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 4</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 4</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 4</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 4</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 4</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 4</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 4</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>104</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>105</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 6</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 6</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 6</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 6</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 6</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 6</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 6</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 6</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 6</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>106</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 7</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 7</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 7</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 7</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 7</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 7</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 7</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 7</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 7</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>107</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 8</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 8</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 8</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 8</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 8</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 8</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 8</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 8</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 8</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>108</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 9</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 9</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 9</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 9</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 9</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 9</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 9</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 9</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 9</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>109</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 10</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 10</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 10</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 10</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 10</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 10</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 10</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 10</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 10</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>110</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 11</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 11</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 11</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 11</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 11</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 11</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 11</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 11</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>111</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 12</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 12</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 12</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 12</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 12</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 12</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 12</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 12</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 12</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>112</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 13</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 13</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 13</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 13</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 13</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 13</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 13</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 13</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 13</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>113</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 14</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 14</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 14</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 14</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 14</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 14</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 14</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 14</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 14</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>114</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Desk</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Main Desktop</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>116</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 17</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 17</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 17</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 17</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 17</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 17</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 17</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 17</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 17</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>117</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 33</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 33</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 33</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 33</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 33</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 33</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 33</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 33</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 33</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>118</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 21</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 21</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 21</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 21</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 21</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 21</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 21</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 21</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 21</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>119</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans1</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans1</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans1</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans1</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans1</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans1</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans1</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans2</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans2</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans3_1</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans3_1</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans3_1</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans3_1</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans3_1</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans3_1</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans3_1</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Storage_1</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N/A_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>121</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans3_1</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans3_1</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans3_1</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans3_1</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans3_1</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans3_1</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beans3_1</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Storage</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>122</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added function to run custom query on database
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -776,12 +776,12 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 7</t>
+          <t xml:space="preserve"> Storage</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 7</t>
+          <t xml:space="preserve"> N/A</t>
         </is>
       </c>
     </row>
@@ -1452,12 +1452,12 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Storage_1</t>
+          <t xml:space="preserve"> Storage</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> N/A_1</t>
+          <t xml:space="preserve"> N/A</t>
         </is>
       </c>
     </row>
@@ -1562,6 +1562,318 @@
       <c r="J22" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 24</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 24</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 24</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 24</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 24</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 24</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 24</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 24</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 24</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>124</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 25</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 25</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 25</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 25</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 25</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 25</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 25</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 25</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 25</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>125</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 26</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 26</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 26</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 26</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 26</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 26</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 26</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 26</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 26</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>126</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 27</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 27</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 27</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 27</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 27</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 27</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 27</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 27</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 27</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>127</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 28</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 28</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 28</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 28</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 28</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 28</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 28</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 28</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 28</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>128</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 29</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 29</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 29</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 29</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 29</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 29</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 29</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 29</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 29</t>
         </is>
       </c>
     </row>

</xml_diff>